<commit_message>
AH | add pws dusun tempate
</commit_message>
<xml_diff>
--- a/application/download/pws_template/template_pws_amp.xlsx
+++ b/application/download/pws_template/template_pws_amp.xlsx
@@ -381,8 +381,6 @@
     <xf numFmtId="1" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -400,6 +398,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -440,7 +441,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -747,8 +751,8 @@
   </sheetPr>
   <dimension ref="A1:AMK72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -784,11 +788,11 @@
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
-      <c r="X1" s="52" t="s">
+      <c r="X1" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
       <c r="ALY1"/>
       <c r="ALZ1"/>
       <c r="AMA1"/>
@@ -972,46 +976,46 @@
       <c r="AMK6"/>
     </row>
     <row r="7" spans="1:1025" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="50"/>
-      <c r="P7" s="50"/>
-      <c r="Q7" s="50"/>
-      <c r="R7" s="50"/>
-      <c r="S7" s="50"/>
-      <c r="T7" s="50"/>
-      <c r="U7" s="50"/>
-      <c r="V7" s="50"/>
-      <c r="W7" s="50"/>
-      <c r="X7" s="50"/>
-      <c r="Y7" s="50"/>
-      <c r="Z7" s="51"/>
-      <c r="AA7" s="44" t="s">
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="49"/>
+      <c r="R7" s="49"/>
+      <c r="S7" s="49"/>
+      <c r="T7" s="49"/>
+      <c r="U7" s="49"/>
+      <c r="V7" s="49"/>
+      <c r="W7" s="49"/>
+      <c r="X7" s="49"/>
+      <c r="Y7" s="49"/>
+      <c r="Z7" s="50"/>
+      <c r="AA7" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="AB7" s="45"/>
-      <c r="AC7" s="44" t="s">
+      <c r="AB7" s="44"/>
+      <c r="AC7" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="AD7" s="45"/>
+      <c r="AD7" s="44"/>
       <c r="ALS7"/>
       <c r="ALT7"/>
       <c r="ALU7"/>
@@ -1033,48 +1037,48 @@
       <c r="AMK7"/>
     </row>
     <row r="8" spans="1:1025" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="41"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="37" t="s">
+      <c r="A8" s="40"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37" t="s">
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37" t="s">
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37" t="s">
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="37"/>
-      <c r="R8" s="37"/>
-      <c r="S8" s="37" t="s">
+      <c r="P8" s="36"/>
+      <c r="Q8" s="36"/>
+      <c r="R8" s="36"/>
+      <c r="S8" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="T8" s="37"/>
-      <c r="U8" s="37"/>
-      <c r="V8" s="37"/>
-      <c r="W8" s="37" t="s">
+      <c r="T8" s="36"/>
+      <c r="U8" s="36"/>
+      <c r="V8" s="36"/>
+      <c r="W8" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="X8" s="37"/>
-      <c r="Y8" s="37"/>
-      <c r="Z8" s="37"/>
-      <c r="AA8" s="46"/>
-      <c r="AB8" s="47"/>
-      <c r="AC8" s="46"/>
-      <c r="AD8" s="47"/>
+      <c r="X8" s="36"/>
+      <c r="Y8" s="36"/>
+      <c r="Z8" s="36"/>
+      <c r="AA8" s="45"/>
+      <c r="AB8" s="46"/>
+      <c r="AC8" s="45"/>
+      <c r="AD8" s="46"/>
       <c r="ALQ8"/>
       <c r="ALR8"/>
       <c r="ALS8"/>
@@ -1098,146 +1102,146 @@
       <c r="AMK8"/>
     </row>
     <row r="9" spans="1:1025" s="23" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="41"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="37" t="s">
+      <c r="A9" s="40"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37" t="s">
+      <c r="D9" s="36"/>
+      <c r="E9" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37" t="s">
+      <c r="F9" s="36"/>
+      <c r="G9" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37" t="s">
+      <c r="H9" s="36"/>
+      <c r="I9" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37" t="s">
+      <c r="J9" s="36"/>
+      <c r="K9" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37" t="s">
+      <c r="L9" s="36"/>
+      <c r="M9" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37" t="s">
+      <c r="N9" s="36"/>
+      <c r="O9" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="P9" s="37"/>
-      <c r="Q9" s="37" t="s">
+      <c r="P9" s="36"/>
+      <c r="Q9" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="R9" s="37"/>
-      <c r="S9" s="37" t="s">
+      <c r="R9" s="36"/>
+      <c r="S9" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="T9" s="37"/>
-      <c r="U9" s="37" t="s">
+      <c r="T9" s="36"/>
+      <c r="U9" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="V9" s="37"/>
-      <c r="W9" s="37" t="s">
+      <c r="V9" s="36"/>
+      <c r="W9" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="X9" s="37"/>
-      <c r="Y9" s="37" t="s">
+      <c r="X9" s="36"/>
+      <c r="Y9" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="Z9" s="37"/>
-      <c r="AA9" s="48"/>
-      <c r="AB9" s="49"/>
-      <c r="AC9" s="48"/>
-      <c r="AD9" s="49"/>
+      <c r="Z9" s="36"/>
+      <c r="AA9" s="47"/>
+      <c r="AB9" s="48"/>
+      <c r="AC9" s="47"/>
+      <c r="AD9" s="48"/>
     </row>
     <row r="10" spans="1:1025" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="41"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="31" t="s">
+      <c r="A10" s="40"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="31" t="s">
+      <c r="F10" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="31" t="s">
+      <c r="G10" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="31" t="s">
+      <c r="I10" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="31" t="s">
+      <c r="J10" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="31" t="s">
+      <c r="K10" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="31" t="s">
+      <c r="L10" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="M10" s="31" t="s">
+      <c r="M10" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="N10" s="31" t="s">
+      <c r="N10" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="31" t="s">
+      <c r="O10" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="P10" s="31" t="s">
+      <c r="P10" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="Q10" s="31" t="s">
+      <c r="Q10" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="R10" s="31" t="s">
+      <c r="R10" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="S10" s="31" t="s">
+      <c r="S10" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="T10" s="31" t="s">
+      <c r="T10" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="U10" s="31" t="s">
+      <c r="U10" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="V10" s="31" t="s">
+      <c r="V10" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="W10" s="31" t="s">
+      <c r="W10" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="X10" s="31" t="s">
+      <c r="X10" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="Y10" s="31" t="s">
+      <c r="Y10" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="Z10" s="31" t="s">
+      <c r="Z10" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="AA10" s="31" t="s">
+      <c r="AA10" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="AB10" s="31" t="s">
+      <c r="AB10" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="AC10" s="31" t="s">
+      <c r="AC10" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="AD10" s="31" t="s">
+      <c r="AD10" s="29" t="s">
         <v>14</v>
       </c>
       <c r="ALQ10"/>
@@ -1269,88 +1273,88 @@
       <c r="B11" s="26">
         <v>2</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C11" s="31">
         <v>3</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11" s="31">
         <v>4</v>
       </c>
-      <c r="E11" s="33">
+      <c r="E11" s="31">
         <v>5</v>
       </c>
-      <c r="F11" s="33">
-        <v>6</v>
-      </c>
-      <c r="G11" s="33">
+      <c r="F11" s="31">
+        <v>6</v>
+      </c>
+      <c r="G11" s="31">
         <v>7</v>
       </c>
-      <c r="H11" s="33">
+      <c r="H11" s="31">
         <v>8</v>
       </c>
-      <c r="I11" s="33">
+      <c r="I11" s="31">
         <v>9</v>
       </c>
-      <c r="J11" s="34">
+      <c r="J11" s="32">
         <v>10</v>
       </c>
-      <c r="K11" s="34">
+      <c r="K11" s="32">
         <v>11</v>
       </c>
-      <c r="L11" s="33">
+      <c r="L11" s="31">
         <v>12</v>
       </c>
-      <c r="M11" s="33">
+      <c r="M11" s="31">
         <v>13</v>
       </c>
-      <c r="N11" s="33">
+      <c r="N11" s="31">
         <v>14</v>
       </c>
-      <c r="O11" s="34">
+      <c r="O11" s="32">
         <v>15</v>
       </c>
-      <c r="P11" s="34">
+      <c r="P11" s="32">
         <v>16</v>
       </c>
-      <c r="Q11" s="33">
+      <c r="Q11" s="31">
         <v>17</v>
       </c>
-      <c r="R11" s="33">
+      <c r="R11" s="31">
         <v>18</v>
       </c>
-      <c r="S11" s="33">
+      <c r="S11" s="31">
         <v>19</v>
       </c>
-      <c r="T11" s="34">
+      <c r="T11" s="32">
         <v>20</v>
       </c>
-      <c r="U11" s="34">
+      <c r="U11" s="32">
         <v>21</v>
       </c>
-      <c r="V11" s="33">
+      <c r="V11" s="31">
         <v>22</v>
       </c>
-      <c r="W11" s="33">
+      <c r="W11" s="31">
         <v>23</v>
       </c>
-      <c r="X11" s="33">
+      <c r="X11" s="31">
         <v>24</v>
       </c>
-      <c r="Y11" s="34">
+      <c r="Y11" s="32">
         <v>25</v>
       </c>
-      <c r="Z11" s="34">
+      <c r="Z11" s="32">
         <v>26</v>
       </c>
-      <c r="AA11" s="34">
+      <c r="AA11" s="32">
         <v>27</v>
       </c>
-      <c r="AB11" s="34">
+      <c r="AB11" s="32">
         <v>28</v>
       </c>
-      <c r="AC11" s="34">
+      <c r="AC11" s="32">
         <v>29</v>
       </c>
-      <c r="AD11" s="34">
+      <c r="AD11" s="32">
         <v>30</v>
       </c>
       <c r="ALQ11"/>
@@ -1378,13 +1382,13 @@
     <row r="12" spans="1:1025" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27"/>
       <c r="B12" s="28"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
       <c r="J12" s="24"/>
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
@@ -1402,10 +1406,10 @@
       <c r="X12" s="24"/>
       <c r="Y12" s="24"/>
       <c r="Z12" s="24"/>
-      <c r="AA12" s="35"/>
-      <c r="AB12" s="35"/>
-      <c r="AC12" s="35"/>
-      <c r="AD12" s="35"/>
+      <c r="AA12" s="33"/>
+      <c r="AB12" s="33"/>
+      <c r="AC12" s="33"/>
+      <c r="AD12" s="33"/>
       <c r="ALQ12"/>
       <c r="ALR12"/>
       <c r="ALS12"/>
@@ -1431,13 +1435,13 @@
     <row r="13" spans="1:1025" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27"/>
       <c r="B13" s="28"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
       <c r="J13" s="24"/>
       <c r="K13" s="24"/>
       <c r="L13" s="24"/>
@@ -1455,10 +1459,10 @@
       <c r="X13" s="24"/>
       <c r="Y13" s="24"/>
       <c r="Z13" s="24"/>
-      <c r="AA13" s="35"/>
-      <c r="AB13" s="35"/>
-      <c r="AC13" s="35"/>
-      <c r="AD13" s="35"/>
+      <c r="AA13" s="33"/>
+      <c r="AB13" s="33"/>
+      <c r="AC13" s="33"/>
+      <c r="AD13" s="33"/>
       <c r="ALQ13"/>
       <c r="ALR13"/>
       <c r="ALS13"/>
@@ -1484,13 +1488,13 @@
     <row r="14" spans="1:1025" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
       <c r="B14" s="28"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
       <c r="J14" s="24"/>
       <c r="K14" s="24"/>
       <c r="L14" s="24"/>
@@ -1508,10 +1512,10 @@
       <c r="X14" s="24"/>
       <c r="Y14" s="24"/>
       <c r="Z14" s="24"/>
-      <c r="AA14" s="35"/>
-      <c r="AB14" s="35"/>
-      <c r="AC14" s="35"/>
-      <c r="AD14" s="35"/>
+      <c r="AA14" s="33"/>
+      <c r="AB14" s="33"/>
+      <c r="AC14" s="33"/>
+      <c r="AD14" s="33"/>
       <c r="ALQ14"/>
       <c r="ALR14"/>
       <c r="ALS14"/>
@@ -1537,365 +1541,365 @@
     <row r="15" spans="1:1025" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="27"/>
       <c r="B15" s="28"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="32"/>
-      <c r="R15" s="32"/>
-      <c r="S15" s="32"/>
-      <c r="T15" s="32"/>
-      <c r="U15" s="32"/>
-      <c r="V15" s="32"/>
-      <c r="W15" s="32"/>
-      <c r="X15" s="32"/>
-      <c r="Y15" s="32"/>
-      <c r="Z15" s="32"/>
-      <c r="AA15" s="35"/>
-      <c r="AB15" s="35"/>
-      <c r="AC15" s="35"/>
-      <c r="AD15" s="35"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="30"/>
+      <c r="U15" s="30"/>
+      <c r="V15" s="30"/>
+      <c r="W15" s="30"/>
+      <c r="X15" s="30"/>
+      <c r="Y15" s="30"/>
+      <c r="Z15" s="30"/>
+      <c r="AA15" s="33"/>
+      <c r="AB15" s="33"/>
+      <c r="AC15" s="33"/>
+      <c r="AD15" s="33"/>
     </row>
     <row r="16" spans="1:1025" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
       <c r="B16" s="28"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="32"/>
-      <c r="S16" s="32"/>
-      <c r="T16" s="32"/>
-      <c r="U16" s="32"/>
-      <c r="V16" s="32"/>
-      <c r="W16" s="32"/>
-      <c r="X16" s="32"/>
-      <c r="Y16" s="32"/>
-      <c r="Z16" s="32"/>
-      <c r="AA16" s="35"/>
-      <c r="AB16" s="35"/>
-      <c r="AC16" s="35"/>
-      <c r="AD16" s="35"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="30"/>
+      <c r="T16" s="30"/>
+      <c r="U16" s="30"/>
+      <c r="V16" s="30"/>
+      <c r="W16" s="30"/>
+      <c r="X16" s="30"/>
+      <c r="Y16" s="30"/>
+      <c r="Z16" s="30"/>
+      <c r="AA16" s="33"/>
+      <c r="AB16" s="33"/>
+      <c r="AC16" s="33"/>
+      <c r="AD16" s="33"/>
     </row>
     <row r="17" spans="1:1025" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="27"/>
       <c r="B17" s="28"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="32"/>
-      <c r="Q17" s="32"/>
-      <c r="R17" s="32"/>
-      <c r="S17" s="32"/>
-      <c r="T17" s="32"/>
-      <c r="U17" s="32"/>
-      <c r="V17" s="32"/>
-      <c r="W17" s="32"/>
-      <c r="X17" s="32"/>
-      <c r="Y17" s="32"/>
-      <c r="Z17" s="32"/>
-      <c r="AA17" s="35"/>
-      <c r="AB17" s="35"/>
-      <c r="AC17" s="35"/>
-      <c r="AD17" s="35"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="30"/>
+      <c r="R17" s="30"/>
+      <c r="S17" s="30"/>
+      <c r="T17" s="30"/>
+      <c r="U17" s="30"/>
+      <c r="V17" s="30"/>
+      <c r="W17" s="30"/>
+      <c r="X17" s="30"/>
+      <c r="Y17" s="30"/>
+      <c r="Z17" s="30"/>
+      <c r="AA17" s="33"/>
+      <c r="AB17" s="33"/>
+      <c r="AC17" s="33"/>
+      <c r="AD17" s="33"/>
     </row>
     <row r="18" spans="1:1025" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="27"/>
       <c r="B18" s="28"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="32"/>
-      <c r="O18" s="32"/>
-      <c r="P18" s="32"/>
-      <c r="Q18" s="32"/>
-      <c r="R18" s="32"/>
-      <c r="S18" s="32"/>
-      <c r="T18" s="32"/>
-      <c r="U18" s="32"/>
-      <c r="V18" s="32"/>
-      <c r="W18" s="32"/>
-      <c r="X18" s="32"/>
-      <c r="Y18" s="32"/>
-      <c r="Z18" s="32"/>
-      <c r="AA18" s="35"/>
-      <c r="AB18" s="35"/>
-      <c r="AC18" s="35"/>
-      <c r="AD18" s="35"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="30"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="30"/>
+      <c r="U18" s="30"/>
+      <c r="V18" s="30"/>
+      <c r="W18" s="30"/>
+      <c r="X18" s="30"/>
+      <c r="Y18" s="30"/>
+      <c r="Z18" s="30"/>
+      <c r="AA18" s="33"/>
+      <c r="AB18" s="33"/>
+      <c r="AC18" s="33"/>
+      <c r="AD18" s="33"/>
     </row>
     <row r="19" spans="1:1025" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="27"/>
       <c r="B19" s="28"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="32"/>
-      <c r="R19" s="32"/>
-      <c r="S19" s="32"/>
-      <c r="T19" s="32"/>
-      <c r="U19" s="32"/>
-      <c r="V19" s="32"/>
-      <c r="W19" s="32"/>
-      <c r="X19" s="32"/>
-      <c r="Y19" s="32"/>
-      <c r="Z19" s="32"/>
-      <c r="AA19" s="35"/>
-      <c r="AB19" s="35"/>
-      <c r="AC19" s="35"/>
-      <c r="AD19" s="35"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="30"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="30"/>
+      <c r="R19" s="30"/>
+      <c r="S19" s="30"/>
+      <c r="T19" s="30"/>
+      <c r="U19" s="30"/>
+      <c r="V19" s="30"/>
+      <c r="W19" s="30"/>
+      <c r="X19" s="30"/>
+      <c r="Y19" s="30"/>
+      <c r="Z19" s="30"/>
+      <c r="AA19" s="33"/>
+      <c r="AB19" s="33"/>
+      <c r="AC19" s="33"/>
+      <c r="AD19" s="33"/>
     </row>
     <row r="20" spans="1:1025" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
       <c r="B20" s="28"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="32"/>
-      <c r="R20" s="32"/>
-      <c r="S20" s="32"/>
-      <c r="T20" s="32"/>
-      <c r="U20" s="32"/>
-      <c r="V20" s="32"/>
-      <c r="W20" s="32"/>
-      <c r="X20" s="32"/>
-      <c r="Y20" s="32"/>
-      <c r="Z20" s="32"/>
-      <c r="AA20" s="35"/>
-      <c r="AB20" s="35"/>
-      <c r="AC20" s="35"/>
-      <c r="AD20" s="35"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="30"/>
+      <c r="R20" s="30"/>
+      <c r="S20" s="30"/>
+      <c r="T20" s="30"/>
+      <c r="U20" s="30"/>
+      <c r="V20" s="30"/>
+      <c r="W20" s="30"/>
+      <c r="X20" s="30"/>
+      <c r="Y20" s="30"/>
+      <c r="Z20" s="30"/>
+      <c r="AA20" s="33"/>
+      <c r="AB20" s="33"/>
+      <c r="AC20" s="33"/>
+      <c r="AD20" s="33"/>
     </row>
     <row r="21" spans="1:1025" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="27"/>
       <c r="B21" s="28"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="32"/>
-      <c r="Q21" s="32"/>
-      <c r="R21" s="32"/>
-      <c r="S21" s="32"/>
-      <c r="T21" s="32"/>
-      <c r="U21" s="32"/>
-      <c r="V21" s="32"/>
-      <c r="W21" s="32"/>
-      <c r="X21" s="32"/>
-      <c r="Y21" s="32"/>
-      <c r="Z21" s="32"/>
-      <c r="AA21" s="35"/>
-      <c r="AB21" s="35"/>
-      <c r="AC21" s="35"/>
-      <c r="AD21" s="35"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="30"/>
+      <c r="R21" s="30"/>
+      <c r="S21" s="30"/>
+      <c r="T21" s="30"/>
+      <c r="U21" s="30"/>
+      <c r="V21" s="30"/>
+      <c r="W21" s="30"/>
+      <c r="X21" s="30"/>
+      <c r="Y21" s="30"/>
+      <c r="Z21" s="30"/>
+      <c r="AA21" s="33"/>
+      <c r="AB21" s="33"/>
+      <c r="AC21" s="33"/>
+      <c r="AD21" s="33"/>
     </row>
     <row r="22" spans="1:1025" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="27"/>
       <c r="B22" s="28"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="32"/>
-      <c r="L22" s="32"/>
-      <c r="M22" s="32"/>
-      <c r="N22" s="32"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="32"/>
-      <c r="Q22" s="32"/>
-      <c r="R22" s="32"/>
-      <c r="S22" s="32"/>
-      <c r="T22" s="32"/>
-      <c r="U22" s="32"/>
-      <c r="V22" s="32"/>
-      <c r="W22" s="32"/>
-      <c r="X22" s="32"/>
-      <c r="Y22" s="32"/>
-      <c r="Z22" s="32"/>
-      <c r="AA22" s="35"/>
-      <c r="AB22" s="35"/>
-      <c r="AC22" s="35"/>
-      <c r="AD22" s="35"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="30"/>
+      <c r="R22" s="30"/>
+      <c r="S22" s="30"/>
+      <c r="T22" s="30"/>
+      <c r="U22" s="30"/>
+      <c r="V22" s="30"/>
+      <c r="W22" s="30"/>
+      <c r="X22" s="30"/>
+      <c r="Y22" s="30"/>
+      <c r="Z22" s="30"/>
+      <c r="AA22" s="33"/>
+      <c r="AB22" s="33"/>
+      <c r="AC22" s="33"/>
+      <c r="AD22" s="33"/>
     </row>
     <row r="23" spans="1:1025" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
       <c r="B23" s="28"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="32"/>
-      <c r="M23" s="32"/>
-      <c r="N23" s="32"/>
-      <c r="O23" s="32"/>
-      <c r="P23" s="32"/>
-      <c r="Q23" s="32"/>
-      <c r="R23" s="32"/>
-      <c r="S23" s="32"/>
-      <c r="T23" s="32"/>
-      <c r="U23" s="32"/>
-      <c r="V23" s="32"/>
-      <c r="W23" s="32"/>
-      <c r="X23" s="32"/>
-      <c r="Y23" s="32"/>
-      <c r="Z23" s="32"/>
-      <c r="AA23" s="35"/>
-      <c r="AB23" s="35"/>
-      <c r="AC23" s="35"/>
-      <c r="AD23" s="35"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="30"/>
+      <c r="R23" s="30"/>
+      <c r="S23" s="30"/>
+      <c r="T23" s="30"/>
+      <c r="U23" s="30"/>
+      <c r="V23" s="30"/>
+      <c r="W23" s="30"/>
+      <c r="X23" s="30"/>
+      <c r="Y23" s="30"/>
+      <c r="Z23" s="30"/>
+      <c r="AA23" s="33"/>
+      <c r="AB23" s="33"/>
+      <c r="AC23" s="33"/>
+      <c r="AD23" s="33"/>
     </row>
     <row r="24" spans="1:1025" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
       <c r="B24" s="28"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="32"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="32"/>
-      <c r="Q24" s="32"/>
-      <c r="R24" s="32"/>
-      <c r="S24" s="32"/>
-      <c r="T24" s="32"/>
-      <c r="U24" s="32"/>
-      <c r="V24" s="32"/>
-      <c r="W24" s="32"/>
-      <c r="X24" s="32"/>
-      <c r="Y24" s="32"/>
-      <c r="Z24" s="32"/>
-      <c r="AA24" s="35"/>
-      <c r="AB24" s="35"/>
-      <c r="AC24" s="35"/>
-      <c r="AD24" s="35"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="30"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="30"/>
+      <c r="T24" s="30"/>
+      <c r="U24" s="30"/>
+      <c r="V24" s="30"/>
+      <c r="W24" s="30"/>
+      <c r="X24" s="30"/>
+      <c r="Y24" s="30"/>
+      <c r="Z24" s="30"/>
+      <c r="AA24" s="33"/>
+      <c r="AB24" s="33"/>
+      <c r="AC24" s="33"/>
+      <c r="AD24" s="33"/>
     </row>
     <row r="25" spans="1:1025" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
       <c r="B25" s="28"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="32"/>
-      <c r="O25" s="32"/>
-      <c r="P25" s="32"/>
-      <c r="Q25" s="32"/>
-      <c r="R25" s="32"/>
-      <c r="S25" s="32"/>
-      <c r="T25" s="32"/>
-      <c r="U25" s="32"/>
-      <c r="V25" s="32"/>
-      <c r="W25" s="32"/>
-      <c r="X25" s="32"/>
-      <c r="Y25" s="32"/>
-      <c r="Z25" s="32"/>
-      <c r="AA25" s="35"/>
-      <c r="AB25" s="35"/>
-      <c r="AC25" s="35"/>
-      <c r="AD25" s="35"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="30"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="30"/>
+      <c r="P25" s="30"/>
+      <c r="Q25" s="30"/>
+      <c r="R25" s="30"/>
+      <c r="S25" s="30"/>
+      <c r="T25" s="30"/>
+      <c r="U25" s="30"/>
+      <c r="V25" s="30"/>
+      <c r="W25" s="30"/>
+      <c r="X25" s="30"/>
+      <c r="Y25" s="30"/>
+      <c r="Z25" s="30"/>
+      <c r="AA25" s="33"/>
+      <c r="AB25" s="33"/>
+      <c r="AC25" s="33"/>
+      <c r="AD25" s="33"/>
     </row>
     <row r="26" spans="1:1025" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
       <c r="B26" s="28"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
       <c r="J26" s="24"/>
       <c r="K26" s="24"/>
       <c r="L26" s="24"/>
@@ -1913,10 +1917,10 @@
       <c r="X26" s="24"/>
       <c r="Y26" s="24"/>
       <c r="Z26" s="24"/>
-      <c r="AA26" s="35"/>
-      <c r="AB26" s="35"/>
-      <c r="AC26" s="35"/>
-      <c r="AD26" s="35"/>
+      <c r="AA26" s="33"/>
+      <c r="AB26" s="33"/>
+      <c r="AC26" s="33"/>
+      <c r="AD26" s="33"/>
       <c r="ALQ26"/>
       <c r="ALR26"/>
       <c r="ALS26"/>
@@ -1942,13 +1946,13 @@
     <row r="27" spans="1:1025" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="27"/>
       <c r="B27" s="28"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
       <c r="J27" s="24"/>
       <c r="K27" s="24"/>
       <c r="L27" s="24"/>
@@ -1966,10 +1970,10 @@
       <c r="X27" s="24"/>
       <c r="Y27" s="24"/>
       <c r="Z27" s="24"/>
-      <c r="AA27" s="35"/>
-      <c r="AB27" s="35"/>
-      <c r="AC27" s="35"/>
-      <c r="AD27" s="35"/>
+      <c r="AA27" s="33"/>
+      <c r="AB27" s="33"/>
+      <c r="AC27" s="33"/>
+      <c r="AD27" s="33"/>
       <c r="ALQ27"/>
       <c r="ALR27"/>
       <c r="ALS27"/>
@@ -1995,13 +1999,13 @@
     <row r="28" spans="1:1025" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="27"/>
       <c r="B28" s="28"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
       <c r="J28" s="24"/>
       <c r="K28" s="24"/>
       <c r="L28" s="24"/>
@@ -2019,10 +2023,10 @@
       <c r="X28" s="24"/>
       <c r="Y28" s="24"/>
       <c r="Z28" s="24"/>
-      <c r="AA28" s="35"/>
-      <c r="AB28" s="35"/>
-      <c r="AC28" s="35"/>
-      <c r="AD28" s="35"/>
+      <c r="AA28" s="33"/>
+      <c r="AB28" s="33"/>
+      <c r="AC28" s="33"/>
+      <c r="AD28" s="33"/>
       <c r="ALQ28"/>
       <c r="ALR28"/>
       <c r="ALS28"/>
@@ -2048,13 +2052,13 @@
     <row r="29" spans="1:1025" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="27"/>
       <c r="B29" s="28"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
       <c r="J29" s="24"/>
       <c r="K29" s="24"/>
       <c r="L29" s="24"/>
@@ -2072,10 +2076,10 @@
       <c r="X29" s="24"/>
       <c r="Y29" s="24"/>
       <c r="Z29" s="24"/>
-      <c r="AA29" s="35"/>
-      <c r="AB29" s="35"/>
-      <c r="AC29" s="35"/>
-      <c r="AD29" s="35"/>
+      <c r="AA29" s="33"/>
+      <c r="AB29" s="33"/>
+      <c r="AC29" s="33"/>
+      <c r="AD29" s="33"/>
       <c r="ALQ29"/>
       <c r="ALR29"/>
       <c r="ALS29"/>
@@ -2101,13 +2105,13 @@
     <row r="30" spans="1:1025" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="27"/>
       <c r="B30" s="28"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
       <c r="J30" s="24"/>
       <c r="K30" s="24"/>
       <c r="L30" s="24"/>
@@ -2125,10 +2129,10 @@
       <c r="X30" s="24"/>
       <c r="Y30" s="24"/>
       <c r="Z30" s="24"/>
-      <c r="AA30" s="35"/>
-      <c r="AB30" s="35"/>
-      <c r="AC30" s="35"/>
-      <c r="AD30" s="35"/>
+      <c r="AA30" s="33"/>
+      <c r="AB30" s="33"/>
+      <c r="AC30" s="33"/>
+      <c r="AD30" s="33"/>
       <c r="ALQ30"/>
       <c r="ALR30"/>
       <c r="ALS30"/>
@@ -2154,13 +2158,13 @@
     <row r="31" spans="1:1025" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="27"/>
       <c r="B31" s="28"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
       <c r="J31" s="24"/>
       <c r="K31" s="24"/>
       <c r="L31" s="24"/>
@@ -2178,10 +2182,10 @@
       <c r="X31" s="24"/>
       <c r="Y31" s="24"/>
       <c r="Z31" s="24"/>
-      <c r="AA31" s="35"/>
-      <c r="AB31" s="35"/>
-      <c r="AC31" s="35"/>
-      <c r="AD31" s="35"/>
+      <c r="AA31" s="33"/>
+      <c r="AB31" s="33"/>
+      <c r="AC31" s="33"/>
+      <c r="AD31" s="33"/>
       <c r="ALQ31"/>
       <c r="ALR31"/>
       <c r="ALS31"/>
@@ -2207,13 +2211,13 @@
     <row r="32" spans="1:1025" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="27"/>
       <c r="B32" s="28"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
       <c r="J32" s="24"/>
       <c r="K32" s="24"/>
       <c r="L32" s="24"/>
@@ -2231,10 +2235,10 @@
       <c r="X32" s="24"/>
       <c r="Y32" s="24"/>
       <c r="Z32" s="24"/>
-      <c r="AA32" s="35"/>
-      <c r="AB32" s="35"/>
-      <c r="AC32" s="35"/>
-      <c r="AD32" s="35"/>
+      <c r="AA32" s="33"/>
+      <c r="AB32" s="33"/>
+      <c r="AC32" s="33"/>
+      <c r="AD32" s="33"/>
       <c r="ALQ32"/>
       <c r="ALR32"/>
       <c r="ALS32"/>
@@ -2260,13 +2264,13 @@
     <row r="33" spans="1:1025" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="27"/>
       <c r="B33" s="28"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
       <c r="J33" s="24"/>
       <c r="K33" s="24"/>
       <c r="L33" s="24"/>
@@ -2284,10 +2288,10 @@
       <c r="X33" s="24"/>
       <c r="Y33" s="24"/>
       <c r="Z33" s="24"/>
-      <c r="AA33" s="35"/>
-      <c r="AB33" s="35"/>
-      <c r="AC33" s="35"/>
-      <c r="AD33" s="35"/>
+      <c r="AA33" s="33"/>
+      <c r="AB33" s="33"/>
+      <c r="AC33" s="33"/>
+      <c r="AD33" s="33"/>
       <c r="ALQ33"/>
       <c r="ALR33"/>
       <c r="ALS33"/>
@@ -2315,13 +2319,13 @@
       <c r="B34" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
       <c r="J34" s="24"/>
       <c r="K34" s="24"/>
       <c r="L34" s="24"/>
@@ -2339,10 +2343,10 @@
       <c r="X34" s="24"/>
       <c r="Y34" s="24"/>
       <c r="Z34" s="24"/>
-      <c r="AA34" s="35"/>
-      <c r="AB34" s="35"/>
-      <c r="AC34" s="35"/>
-      <c r="AD34" s="35"/>
+      <c r="AA34" s="33"/>
+      <c r="AB34" s="33"/>
+      <c r="AC34" s="33"/>
+      <c r="AD34" s="33"/>
       <c r="ALQ34"/>
       <c r="ALR34"/>
       <c r="ALS34"/>
@@ -2370,13 +2374,13 @@
       <c r="B35" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
       <c r="J35" s="24"/>
       <c r="K35" s="24"/>
       <c r="L35" s="24"/>
@@ -2394,10 +2398,10 @@
       <c r="X35" s="24"/>
       <c r="Y35" s="24"/>
       <c r="Z35" s="24"/>
-      <c r="AA35" s="35"/>
-      <c r="AB35" s="35"/>
-      <c r="AC35" s="35"/>
-      <c r="AD35" s="35"/>
+      <c r="AA35" s="33"/>
+      <c r="AB35" s="33"/>
+      <c r="AC35" s="33"/>
+      <c r="AD35" s="33"/>
       <c r="ALQ35"/>
       <c r="ALR35"/>
       <c r="ALS35"/>
@@ -2421,17 +2425,17 @@
       <c r="AMK35"/>
     </row>
     <row r="36" spans="1:1025" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="29"/>
-      <c r="B36" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
+      <c r="A36" s="51"/>
+      <c r="B36" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
       <c r="J36" s="24"/>
       <c r="K36" s="24"/>
       <c r="L36" s="24"/>
@@ -2449,10 +2453,10 @@
       <c r="X36" s="24"/>
       <c r="Y36" s="24"/>
       <c r="Z36" s="24"/>
-      <c r="AA36" s="35"/>
-      <c r="AB36" s="35"/>
-      <c r="AC36" s="35"/>
-      <c r="AD36" s="35"/>
+      <c r="AA36" s="33"/>
+      <c r="AB36" s="33"/>
+      <c r="AC36" s="33"/>
+      <c r="AD36" s="33"/>
       <c r="ALQ36"/>
       <c r="ALR36"/>
       <c r="ALS36"/>
@@ -2476,119 +2480,119 @@
       <c r="AMK36"/>
     </row>
     <row r="37" spans="1:1025" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="38" t="s">
+      <c r="A37" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="39"/>
-      <c r="C37" s="31" t="str">
+      <c r="B37" s="38"/>
+      <c r="C37" s="29" t="str">
         <f>IF(SUM(C12:C36)=0,"-",SUM(C12:C36))</f>
         <v>-</v>
       </c>
-      <c r="D37" s="31" t="str">
+      <c r="D37" s="29" t="str">
         <f t="shared" ref="D37:AD37" si="0">IF(SUM(D12:D36)=0,"-",SUM(D12:D36))</f>
         <v>-</v>
       </c>
-      <c r="E37" s="31" t="str">
+      <c r="E37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="F37" s="31" t="str">
+      <c r="F37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="G37" s="31" t="str">
+      <c r="G37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="H37" s="31" t="str">
+      <c r="H37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="I37" s="31" t="str">
+      <c r="I37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="J37" s="31" t="str">
+      <c r="J37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="K37" s="31" t="str">
+      <c r="K37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="L37" s="31" t="str">
+      <c r="L37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="M37" s="31" t="str">
+      <c r="M37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="N37" s="31" t="str">
+      <c r="N37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="O37" s="31" t="str">
+      <c r="O37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="P37" s="31" t="str">
+      <c r="P37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="Q37" s="31" t="str">
+      <c r="Q37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="R37" s="31" t="str">
+      <c r="R37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="S37" s="31" t="str">
+      <c r="S37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="T37" s="31" t="str">
+      <c r="T37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="U37" s="31" t="str">
+      <c r="U37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="V37" s="31" t="str">
+      <c r="V37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="W37" s="31" t="str">
+      <c r="W37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="X37" s="31" t="str">
+      <c r="X37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="Y37" s="31" t="str">
+      <c r="Y37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="Z37" s="31" t="str">
+      <c r="Z37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="AA37" s="31" t="str">
+      <c r="AA37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="AB37" s="31" t="str">
+      <c r="AB37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="AC37" s="31" t="str">
+      <c r="AC37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="AD37" s="31" t="str">
+      <c r="AD37" s="29" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
@@ -3023,11 +3027,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="X1:Z1"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="B7:B10"/>
     <mergeCell ref="AA7:AB9"/>
     <mergeCell ref="AC7:AD9"/>
     <mergeCell ref="C7:Z7"/>
@@ -3044,6 +3043,11 @@
     <mergeCell ref="Y9:Z9"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="G8:J8"/>
+    <mergeCell ref="X1:Z1"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B7:B10"/>
     <mergeCell ref="K8:N8"/>
     <mergeCell ref="O8:R8"/>
     <mergeCell ref="S8:V8"/>

</xml_diff>